<commit_message>
Fixed several errors in the search. Added targgeted fields to data.xls
</commit_message>
<xml_diff>
--- a/excel-to-json/categories.xlsx
+++ b/excel-to-json/categories.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295B1336-0281-44F2-80C1-C9204F80B67D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489D911A-977F-4920-8B15-952EC6EFA7B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="125">
   <si>
     <t>EN</t>
   </si>
@@ -127,24 +133,6 @@
     <t>cat11</t>
   </si>
   <si>
-    <t>cat22</t>
-  </si>
-  <si>
-    <t>cat33</t>
-  </si>
-  <si>
-    <t>cat44</t>
-  </si>
-  <si>
-    <t>cat21</t>
-  </si>
-  <si>
-    <t>cat31</t>
-  </si>
-  <si>
-    <t>cat41</t>
-  </si>
-  <si>
     <t>Alojamiento</t>
   </si>
   <si>
@@ -286,51 +274,6 @@
     <t>Atención psiquiátrica</t>
   </si>
   <si>
-    <t>cat12</t>
-  </si>
-  <si>
-    <t>cat23</t>
-  </si>
-  <si>
-    <t>cat24</t>
-  </si>
-  <si>
-    <t>cat25</t>
-  </si>
-  <si>
-    <t>cat26</t>
-  </si>
-  <si>
-    <t>cat27</t>
-  </si>
-  <si>
-    <t>cat28</t>
-  </si>
-  <si>
-    <t>cat29</t>
-  </si>
-  <si>
-    <t>cat32</t>
-  </si>
-  <si>
-    <t>cat34</t>
-  </si>
-  <si>
-    <t>cat35</t>
-  </si>
-  <si>
-    <t>cat36</t>
-  </si>
-  <si>
-    <t>cat42</t>
-  </si>
-  <si>
-    <t>cat13</t>
-  </si>
-  <si>
-    <t>cat43</t>
-  </si>
-  <si>
     <t>Clases de español</t>
   </si>
   <si>
@@ -361,15 +304,6 @@
     <t>Internet</t>
   </si>
   <si>
-    <t>cat14</t>
-  </si>
-  <si>
-    <t>cat15</t>
-  </si>
-  <si>
-    <t>cat16</t>
-  </si>
-  <si>
     <t>services[1].key</t>
   </si>
   <si>
@@ -392,6 +326,81 @@
   </si>
   <si>
     <t>services[8].key</t>
+  </si>
+  <si>
+    <t>srv11</t>
+  </si>
+  <si>
+    <t>srv12</t>
+  </si>
+  <si>
+    <t>srv13</t>
+  </si>
+  <si>
+    <t>srv14</t>
+  </si>
+  <si>
+    <t>srv15</t>
+  </si>
+  <si>
+    <t>srv16</t>
+  </si>
+  <si>
+    <t>srv21</t>
+  </si>
+  <si>
+    <t>srv22</t>
+  </si>
+  <si>
+    <t>srv23</t>
+  </si>
+  <si>
+    <t>srv24</t>
+  </si>
+  <si>
+    <t>srv25</t>
+  </si>
+  <si>
+    <t>srv26</t>
+  </si>
+  <si>
+    <t>srv27</t>
+  </si>
+  <si>
+    <t>srv28</t>
+  </si>
+  <si>
+    <t>srv29</t>
+  </si>
+  <si>
+    <t>srv31</t>
+  </si>
+  <si>
+    <t>srv32</t>
+  </si>
+  <si>
+    <t>srv33</t>
+  </si>
+  <si>
+    <t>srv34</t>
+  </si>
+  <si>
+    <t>srv35</t>
+  </si>
+  <si>
+    <t>srv36</t>
+  </si>
+  <si>
+    <t>srv41</t>
+  </si>
+  <si>
+    <t>srv42</t>
+  </si>
+  <si>
+    <t>srv43</t>
+  </si>
+  <si>
+    <t>srv44</t>
   </si>
 </sst>
 </file>
@@ -726,35 +735,35 @@
   <dimension ref="A1:AX12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="9.140625" style="2"/>
-    <col min="16" max="16" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="9.140625" style="2"/>
-    <col min="21" max="21" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="9.140625" style="2"/>
-    <col min="26" max="26" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="9.140625" style="2"/>
-    <col min="31" max="31" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="9.140625" style="2"/>
-    <col min="36" max="36" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="9.140625" style="2"/>
-    <col min="41" max="41" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="45" width="9.140625" style="2"/>
-    <col min="46" max="46" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="34.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="2"/>
+    <col min="6" max="6" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="9.109375" style="2"/>
+    <col min="16" max="16" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="9.109375" style="2"/>
+    <col min="21" max="21" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="9.109375" style="2"/>
+    <col min="26" max="26" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="9.109375" style="2"/>
+    <col min="31" max="31" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="9.109375" style="2"/>
+    <col min="36" max="36" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="9.109375" style="2"/>
+    <col min="41" max="41" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="45" width="9.109375" style="2"/>
+    <col min="46" max="46" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
@@ -789,124 +798,124 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AJ1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AO1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
@@ -926,10 +935,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>10</v>
@@ -941,10 +950,10 @@
         <v>12</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>10</v>
@@ -956,10 +965,10 @@
         <v>12</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>10</v>
@@ -971,10 +980,10 @@
         <v>12</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>10</v>
@@ -986,10 +995,10 @@
         <v>12</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>10</v>
@@ -1001,10 +1010,10 @@
         <v>12</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>10</v>
@@ -1033,130 +1042,130 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="AQ3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU3" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AQ3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AR3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AU3" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="AV3" s="2" t="s">
         <v>10</v>
@@ -1185,10 +1194,10 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -1200,10 +1209,10 @@
         <v>12</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>10</v>
@@ -1215,10 +1224,10 @@
         <v>12</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>10</v>
@@ -1230,10 +1239,10 @@
         <v>12</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>10</v>
@@ -1245,10 +1254,10 @@
         <v>12</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>10</v>
@@ -1260,10 +1269,10 @@
         <v>12</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="AG4" s="2" t="s">
         <v>10</v>
@@ -1292,10 +1301,10 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>10</v>
@@ -1307,10 +1316,10 @@
         <v>12</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>10</v>
@@ -1322,10 +1331,10 @@
         <v>12</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>10</v>
@@ -1337,10 +1346,10 @@
         <v>12</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Reworked data.xlsx to include several sheets. Added specialties to the menu
</commit_message>
<xml_diff>
--- a/excel-to-json/categories.xlsx
+++ b/excel-to-json/categories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489D911A-977F-4920-8B15-952EC6EFA7B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EC652E-24ED-4C65-A425-D51E80BBF7F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -735,35 +735,35 @@
   <dimension ref="A1:AX12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="34.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="2"/>
-    <col min="6" max="6" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="9.109375" style="2"/>
-    <col min="16" max="16" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="9.109375" style="2"/>
-    <col min="21" max="21" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="9.109375" style="2"/>
-    <col min="26" max="26" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="9.109375" style="2"/>
-    <col min="31" max="31" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="9.109375" style="2"/>
-    <col min="36" max="36" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="9.109375" style="2"/>
-    <col min="41" max="41" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="45" width="9.109375" style="2"/>
-    <col min="46" max="46" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="9.140625" style="2"/>
+    <col min="16" max="16" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="9.140625" style="2"/>
+    <col min="21" max="21" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="9.140625" style="2"/>
+    <col min="26" max="26" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="9.140625" style="2"/>
+    <col min="31" max="31" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="9.140625" style="2"/>
+    <col min="36" max="36" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="9.140625" style="2"/>
+    <col min="41" max="41" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="45" width="9.140625" style="2"/>
+    <col min="46" max="46" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">

</xml_diff>